<commit_message>
Test Verion (Po Forecast)
</commit_message>
<xml_diff>
--- a/Sufficient data/forecast_summary_B08F7BHDLY.xlsx
+++ b/Sufficient data/forecast_summary_B08F7BHDLY.xlsx
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" t="n">
         <v>82</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E4" t="n">
         <v>86</v>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E5" t="n">
         <v>87</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E9" t="n">
         <v>85</v>
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E10" t="n">
         <v>84</v>
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E11" t="n">
         <v>80</v>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E14" t="n">
         <v>80</v>
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E15" t="n">
         <v>75</v>
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E16" t="n">
         <v>75</v>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E17" t="n">
         <v>74</v>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1588</t>
+          <t>1612</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>846</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>407</t>
+          <t>415</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>86</t>
         </is>
       </c>
     </row>

</xml_diff>